<commit_message>
reading from excel and putting into list
</commit_message>
<xml_diff>
--- a/house_list.xlsx
+++ b/house_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryandjoseph/Desktop/Projects/py_scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4621152-4F4F-EC46-9EEF-3BC16D800271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09BFDC8-944A-6043-9094-1F76AE0B52A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23720" yWindow="7460" windowWidth="28040" windowHeight="17440" xr2:uid="{DD18D018-7705-974D-BB25-44BD0EBEDE95}"/>
+    <workbookView xWindow="21140" yWindow="1320" windowWidth="28040" windowHeight="17460" xr2:uid="{DD18D018-7705-974D-BB25-44BD0EBEDE95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>James</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Anthony</t>
+  </si>
+  <si>
+    <t>HOUSE_LIST</t>
   </si>
 </sst>
 </file>
@@ -443,69 +446,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57D3128-EF36-E743-B2A8-A338BF657DE7}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>